<commit_message>
Nueva rama con sitio facebook
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hheit\Desktop\hheit\Cursos\Tsoft\Transformacion en Automatizador\RepasoCurso\src\main\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\Java\RepasoCurso-main\RepasoCurso\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>TituloCPs</t>
   </si>
@@ -44,88 +44,43 @@
     <t>Dato005</t>
   </si>
   <si>
-    <t>Dato006</t>
-  </si>
-  <si>
-    <t>Dato007</t>
-  </si>
-  <si>
-    <t>Dato008</t>
-  </si>
-  <si>
-    <t>Dato009</t>
-  </si>
-  <si>
-    <t>Dato010</t>
-  </si>
-  <si>
-    <t>Dato00N</t>
-  </si>
-  <si>
-    <t>CP004</t>
-  </si>
-  <si>
-    <t>CP005</t>
-  </si>
-  <si>
-    <t>CP006</t>
-  </si>
-  <si>
-    <t>CP007</t>
-  </si>
-  <si>
-    <t>CP008</t>
-  </si>
-  <si>
-    <t>CP009</t>
-  </si>
-  <si>
-    <t>CP010</t>
-  </si>
-  <si>
-    <t>CP011</t>
-  </si>
-  <si>
-    <t>CP012</t>
-  </si>
-  <si>
-    <t>CP013</t>
-  </si>
-  <si>
-    <t>CP014</t>
-  </si>
-  <si>
-    <t>CP015</t>
-  </si>
-  <si>
-    <t>CP016</t>
-  </si>
-  <si>
-    <t>CP017</t>
-  </si>
-  <si>
-    <t>CP018</t>
-  </si>
-  <si>
-    <t>CP019</t>
-  </si>
-  <si>
-    <t>CP020</t>
-  </si>
-  <si>
     <t>CP001_login_fallido</t>
   </si>
   <si>
-    <t>CP002_registro_erroneo_rut_faltante</t>
-  </si>
-  <si>
-    <t>CP003_registro_erroneo_correo_faltante</t>
-  </si>
-  <si>
-    <t>algo@algo.com</t>
-  </si>
-  <si>
-    <t>No puedes acceder</t>
+    <t>jisola.tsoft@gmail.com</t>
+  </si>
+  <si>
+    <t>CP002_login_exitoso</t>
+  </si>
+  <si>
+    <t>CP003_cerrar_sesion</t>
+  </si>
+  <si>
+    <t>CP004_modo_oscuro</t>
+  </si>
+  <si>
+    <t>CP005_buscar_persona</t>
+  </si>
+  <si>
+    <t>CP006_enviar_solicitud</t>
+  </si>
+  <si>
+    <t>CP007_cancelar_solicitud</t>
+  </si>
+  <si>
+    <t>CP008_meGusta_pagina</t>
+  </si>
+  <si>
+    <t>CP009_crear_publicacion</t>
+  </si>
+  <si>
+    <t>CP010_crear_historia</t>
+  </si>
+  <si>
+    <t>CP011_enviar_mensaje</t>
+  </si>
+  <si>
+    <t>¿Olvidaste tu contraseña?</t>
   </si>
 </sst>
 </file>
@@ -175,7 +130,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,20 +443,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -520,132 +475,69 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C2">
+        <v>12345678</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2">
-        <v>4234234</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inicio caso de prueba 03
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>TituloCPs</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>¿Olvidaste tu contraseña?</t>
+  </si>
+  <si>
+    <t>Te damos la bienvenida a Facebook, Juan</t>
   </si>
 </sst>
 </file>
@@ -446,7 +449,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,11 +497,26 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>12061990</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>12061990</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -543,6 +561,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se adapto el proyecto para empezar  con el trabajo practico usando la pagina de youtube
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>TituloCPs</t>
   </si>
@@ -122,10 +122,13 @@
     <t>CP003_registro_erroneo_correo_faltante</t>
   </si>
   <si>
-    <t>algo@algo.com</t>
-  </si>
-  <si>
     <t>No puedes acceder</t>
+  </si>
+  <si>
+    <t>hernanheit190@gmail.com</t>
+  </si>
+  <si>
+    <t>Ingenieria21</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,13 +547,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>32</v>
-      </c>
-      <c r="C2">
-        <v>4234234</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se arreglan localizadores en WelcomePage y nombre de metodos
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>TituloCPs</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Te damos la bienvenida a Facebook, Juan</t>
+  </si>
+  <si>
+    <t>Iniciar sesión</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,10 +520,19 @@
       <c r="C4">
         <v>12061990</v>
       </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>12061990</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -563,6 +575,7 @@
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se agrego el caso 008 de dar mg a una pag, se agrego un beforemetod
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\Java\RepasoCurso-main\RepasoCurso\src\main\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hheit\Desktop\hheit\Cursos\Tsoft\Transformacion en Automatizador\RepasoCurso\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>TituloCPs</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Te damos la bienvenida a Facebook, Juan</t>
+  </si>
+  <si>
+    <t>Tsoft</t>
   </si>
 </sst>
 </file>
@@ -133,7 +136,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,10 +452,10 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -542,6 +545,15 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>12061990</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -563,7 +575,9 @@
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregaron los casos 05, 06 y 08
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>TituloCPs</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Tsoft</t>
+  </si>
+  <si>
+    <t>Te gusta</t>
+  </si>
+  <si>
+    <t>juan martin isola</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -131,9 +140,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -452,7 +464,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,16 +542,43 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>12061990</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>12061990</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>12061990</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -553,6 +592,9 @@
       </c>
       <c r="D9" t="s">
         <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -576,8 +618,11 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B9" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se actualizan los CP 4 y 10
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -1,30 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\Java\RepasoCurso-main\RepasoCurso\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF09446-E2B7-40E5-84DB-12304F1D87A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataPrueba" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>TituloCPs</t>
   </si>
@@ -87,12 +96,18 @@
   </si>
   <si>
     <t>Iniciar sesión</t>
+  </si>
+  <si>
+    <t>dark-mode</t>
+  </si>
+  <si>
+    <t>historia de prueba2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -448,11 +463,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,6 +549,9 @@
       <c r="C5">
         <v>12061990</v>
       </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -564,6 +582,15 @@
       <c r="A11" t="s">
         <v>16</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>12061990</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -572,10 +599,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{8FAF5F60-E099-46C4-860B-FF1808079E3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se corrigio un locator del caso 08 y se corrigieron las anotaciones para correr todos los casos
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>TituloCPs</t>
   </si>
@@ -95,7 +95,10 @@
     <t>juan martin isola</t>
   </si>
   <si>
-    <t>true</t>
+    <t>Cancelar solicitud</t>
+  </si>
+  <si>
+    <t>Agregar</t>
   </si>
 </sst>
 </file>
@@ -463,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,6 +581,12 @@
       </c>
       <c r="C8">
         <v>12061990</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ultimos toques de mvn
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\Java\RepasoCurso-main\RepasoCurso\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF09446-E2B7-40E5-84DB-12304F1D87A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A58DC16-BFB0-4ABE-8671-270F767B9C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25830" yWindow="5310" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataPrueba" sheetId="1" r:id="rId1"/>
@@ -467,7 +467,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se corrigieron los conflictos del merge
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\Java\RepasoCurso-main\RepasoCurso\src\main\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hheit\Desktop\Proyecto\RepasoCurso\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A58DC16-BFB0-4ABE-8671-270F767B9C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25830" yWindow="5310" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25830" yWindow="5310" windowWidth="21600" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="DataPrueba" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>TituloCPs</t>
   </si>
@@ -102,12 +101,27 @@
   </si>
   <si>
     <t>historia de prueba2</t>
+  </si>
+  <si>
+    <t>juan martin isola</t>
+  </si>
+  <si>
+    <t>Cancelar solicitud</t>
+  </si>
+  <si>
+    <t>Agregar</t>
+  </si>
+  <si>
+    <t>Tsoft</t>
+  </si>
+  <si>
+    <t>Te gusta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,12 +160,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -463,14 +478,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -557,21 +572,66 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>12061990</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>12061990</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>12061990</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>12061990</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -599,11 +659,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B11" r:id="rId5" xr:uid="{8FAF5F60-E099-46C4-860B-FF1808079E3D}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B11" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId7"/>
+    <hyperlink ref="B8" r:id="rId8"/>
+    <hyperlink ref="B9" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se agrega try catch al espanol y ultimos ajustes
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hheit\Desktop\Proyecto\RepasoCurso\src\main\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\Java\RepasoCurso-main\RepasoCurso\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFE8998-440C-4D23-8625-CA51ED72B607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25830" yWindow="5310" windowWidth="21600" windowHeight="11835"/>
+    <workbookView xWindow="12000" yWindow="3300" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataPrueba" sheetId="1" r:id="rId1"/>
@@ -19,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -115,13 +108,13 @@
     <t>Tsoft</t>
   </si>
   <si>
-    <t>Te gusta</t>
+    <t>Te gusta esta página</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,7 +159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,14 +471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
@@ -659,15 +652,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B11" r:id="rId5"/>
-    <hyperlink ref="B6" r:id="rId6"/>
-    <hyperlink ref="B7" r:id="rId7"/>
-    <hyperlink ref="B8" r:id="rId8"/>
-    <hyperlink ref="B9" r:id="rId9"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B9" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>